<commit_message>
Update rake task with new questions and additional products
</commit_message>
<xml_diff>
--- a/utils/HealthVettedSolutions.xlsx
+++ b/utils/HealthVettedSolutions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
   <si>
     <t>Timestamp</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>Under 50,000 USD (Pilot)</t>
+  </si>
+  <si>
+    <t>Iyewo</t>
+  </si>
+  <si>
+    <t>Less than 1000 (Pilot)</t>
+  </si>
+  <si>
+    <t>Dispensary by Famasi Africa</t>
+  </si>
+  <si>
+    <t>Over 250,000 USD (Mature)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +215,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -359,11 +371,25 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -400,10 +426,28 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -464,7 +508,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA6" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA8" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="27">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="What is the name of the solution" id="2"/>
@@ -1177,6 +1221,148 @@
         <v>35</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="14">
+        <v>45562.44997436342</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA7" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17">
+        <v>45562.452919351854</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA8" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add new solutions to spreadsheet
</commit_message>
<xml_diff>
--- a/utils/HealthVettedSolutions.xlsx
+++ b/utils/HealthVettedSolutions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="87">
   <si>
     <t>Timestamp</t>
   </si>
@@ -254,6 +254,24 @@
   </si>
   <si>
     <t>Medpharma</t>
+  </si>
+  <si>
+    <t>Alô Vida+</t>
+  </si>
+  <si>
+    <t>MedTrack</t>
+  </si>
+  <si>
+    <t>Spes 360</t>
+  </si>
+  <si>
+    <t>Aviro Pocket Clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XanaHealth </t>
+  </si>
+  <si>
+    <t>BetaLife</t>
   </si>
 </sst>
 </file>
@@ -284,7 +302,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -440,25 +458,11 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -519,9 +523,6 @@
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -580,7 +581,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA25" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA31" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="27">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="What is the name of the solution" id="2"/>
@@ -2746,86 +2747,542 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="18">
+      <c r="A25" s="14">
         <v>45568.454662511576</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="19" t="s">
+      <c r="C25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M25" s="19" t="s">
+      <c r="M25" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="N25" s="19" t="s">
+      <c r="N25" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="O25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="P25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="R25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="S25" s="19" t="s">
+      <c r="O25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="T25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="U25" s="19" t="s">
+      <c r="T25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="V25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="W25" s="19" t="s">
+      <c r="V25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W25" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X25" s="19" t="s">
+      <c r="X25" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="Y25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA25" s="20" t="s">
-        <v>28</v>
+      <c r="Y25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA25" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12">
+        <v>45569.53350535879</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="V26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="X26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA26" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="14">
+        <v>45569.69487824074</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="T27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="V27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W27" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X27" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA27" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="12">
+        <v>45572.434264166666</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="V28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="X28" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA28" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="14">
+        <v>45572.626628275466</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z29" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA29" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="12">
+        <v>45572.63018476852</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="T30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="V30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="W30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="X30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA30" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="18">
+        <v>45572.63892673611</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M31" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor update to solution vetting data
</commit_message>
<xml_diff>
--- a/utils/HealthVettedSolutions.xlsx
+++ b/utils/HealthVettedSolutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C787CD7-3634-D74B-9EFA-52D8E09BA744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339EAB0B-79B5-C143-BF21-A2A47BA93852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2840" windowWidth="32420" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="78">
   <si>
     <t>Timestamp</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Afyalytics</t>
+  </si>
+  <si>
+    <t>The S+ Platform</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -273,6 +276,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="3">
@@ -436,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -466,6 +481,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,11 +776,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2054,7 +2072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>45572.626628275466</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>45572.630184768517</v>
       </c>
@@ -2220,7 +2238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>45575.720922118053</v>
       </c>
@@ -2303,7 +2321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>45581.452085462966</v>
       </c>
@@ -2386,7 +2404,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>45581.563527974533</v>
       </c>
@@ -2469,7 +2487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>45581.566317291668</v>
       </c>
@@ -2548,6 +2566,95 @@
       <c r="AA22" s="3" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="11">
+        <v>45587.669074074074</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>